<commit_message>
M+ M- Mx M/ -- added
Initial:  M+ M- Mx M/
</commit_message>
<xml_diff>
--- a/Software/Arduino/Projekte/snc98/Document/Switch_Calculator.xlsx
+++ b/Software/Arduino/Projekte/snc98/Document/Switch_Calculator.xlsx
@@ -18,17 +18,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1591713358" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1591713358" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" keepXLPalette="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1591713358" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1591713358"/>
+      <pm:revision xmlns:pm="smNativeData" day="1600628105" val="978" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1600628105" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" keepXLPalette="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1600628105" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1600628105"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="297">
   <si>
     <t>Ascii</t>
   </si>
@@ -950,7 +950,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -965,7 +965,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -980,7 +980,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="FFFFFF" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="FFFFFF" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -996,7 +996,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="333333" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="333333" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -1012,7 +1012,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="FF9900" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="FF9900" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -1027,7 +1027,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="333399" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="333399" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1043,7 +1043,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -1059,7 +1059,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="7F7F7F" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="7F7F7F" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="220" lang="default" i="1"/>
@@ -1074,7 +1074,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="007F00" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="007F00" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1089,7 +1089,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="993300" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="993300" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1104,7 +1104,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="7F007F" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="7F007F" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1120,7 +1120,7 @@
       <sz val="18"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="003366" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="003366" ulstyle="none">
             <pm:latin face="Cambria" sz="360" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="360" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="360" lang="default" weight="bold"/>
@@ -1136,7 +1136,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="003366" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="003366" ulstyle="none">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="300" lang="default" weight="bold"/>
@@ -1152,7 +1152,7 @@
       <sz val="13"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="003366" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="003366" ulstyle="none">
             <pm:latin face="Calibri" sz="260" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="260" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="260" lang="default" weight="bold"/>
@@ -1168,7 +1168,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="003366" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="003366" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -1183,7 +1183,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="FF9900" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="FF9900" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1198,7 +1198,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="FF0000" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="FF0000" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1214,7 +1214,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591713358" fgClr="FFFFFF" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1600628105" fgClr="FFFFFF" ulstyle="none">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -1236,7 +1236,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00CCCCFF" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00CCCCFF" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1247,7 +1247,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FF99CC" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FF99CC" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1258,7 +1258,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00CCFFCC" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00CCFFCC" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1269,7 +1269,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00CC99FF" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00CC99FF" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1280,7 +1280,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00CCFFFF" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00CCFFFF" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1291,7 +1291,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1302,7 +1302,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="0099CCFF" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="0099CCFF" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1313,7 +1313,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FF8080" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FF8080" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1324,7 +1324,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="0000FF00" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1335,7 +1335,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FFCC00" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FFCC00" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1346,7 +1346,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="000066CC" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="000066CC" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1357,7 +1357,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="007F007F" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="007F007F" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1368,7 +1368,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="0033CCCC" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="0033CCCC" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1379,7 +1379,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FF9900" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FF9900" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1390,7 +1390,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00333399" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00333399" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1401,7 +1401,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1412,7 +1412,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00339966" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00339966" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1423,7 +1423,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FF6600" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FF6600" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1434,7 +1434,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1445,7 +1445,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1456,7 +1456,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1470,7 +1470,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FFFF99" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FFFF99" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1481,7 +1481,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1504,7 +1504,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00999999" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00999999" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1515,7 +1515,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591713358" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1600628105" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1537,7 +1537,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1556,7 +1556,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1575,7 +1575,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1594,7 +1594,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1613,7 +1613,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1632,7 +1632,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1651,7 +1651,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1670,7 +1670,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1689,7 +1689,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1708,7 +1708,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1727,7 +1727,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1746,7 +1746,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1765,7 +1765,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1784,7 +1784,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1803,7 +1803,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1822,7 +1822,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1841,7 +1841,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1860,7 +1860,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1879,7 +1879,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -1898,7 +1898,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="333333"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="333333"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="333333"/>
@@ -1922,7 +1922,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1946,7 +1946,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1970,7 +1970,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="333399"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="333399"/>
           </pm:border>
@@ -1992,7 +1992,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -2011,7 +2011,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="C0C0C0"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="C0C0C0"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="C0C0C0"/>
@@ -2035,7 +2035,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="bottom" type="1" style="0" width="50" dist="20" width2="20" rgb="333399"/>
           </pm:border>
         </ext>
@@ -2056,7 +2056,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="bottom" type="1" style="0" width="50" dist="20" width2="20" rgb="C0C0C0"/>
           </pm:border>
         </ext>
@@ -2077,7 +2077,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="0066CC"/>
           </pm:border>
         </ext>
@@ -2098,7 +2098,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="FF9900"/>
           </pm:border>
         </ext>
@@ -2119,7 +2119,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358">
+          <pm:border xmlns:pm="smNativeData" id="1600628105">
             <pm:line position="top" type="2" style="0" width="20" dist="20" width2="20" rgb="333333"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="333333"/>
             <pm:line position="left" type="2" style="0" width="20" dist="20" width2="20" rgb="333333"/>
@@ -2143,7 +2143,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591713358"/>
+          <pm:border xmlns:pm="smNativeData" id="1600628105"/>
         </ext>
       </extLst>
     </border>
@@ -2311,10 +2311,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1591713358" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1600628105" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1591713358" count="28">
+      <pm:colors xmlns:pm="smNativeData" id="1600628105" count="28">
         <pm:color name="Immergrün" rgb="9999FF"/>
         <pm:color name="Pflaume" rgb="993366"/>
         <pm:color name="Elfenbein" rgb="FFFFCC"/>
@@ -2618,8 +2618,8 @@
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B88" sqref="B88"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F204" sqref="F204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.000000" defaultRowHeight="15.40"/>
@@ -5660,7 +5660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:6">
       <c r="A175">
         <f>A174+1</f>
         <v>174</v>
@@ -5674,8 +5674,11 @@
       <c r="D175" s="47" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="F175" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176">
         <f>A175+1</f>
         <v>175</v>
@@ -5690,8 +5693,11 @@
       <c r="D176" s="47" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="177" spans="1:4">
+      <c r="F176" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
       <c r="A177">
         <f>A176+1</f>
         <v>176</v>
@@ -5706,8 +5712,11 @@
       <c r="D177" s="47" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="178" spans="1:4">
+      <c r="F177" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178">
         <f>A177+1</f>
         <v>177</v>
@@ -5722,8 +5731,11 @@
       <c r="D178" s="47" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="179" spans="1:4">
+      <c r="F178" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179">
         <f>A178+1</f>
         <v>178</v>
@@ -5738,8 +5750,11 @@
       <c r="D179" s="47" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="F179" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180">
         <f>A179+1</f>
         <v>179</v>
@@ -5754,8 +5769,11 @@
       <c r="D180" s="47" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="181" spans="1:4">
+      <c r="F180" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181">
         <f>A180+1</f>
         <v>180</v>
@@ -5770,8 +5788,11 @@
       <c r="D181" s="47" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="182" spans="1:4">
+      <c r="F181" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182">
         <f>A181+1</f>
         <v>181</v>
@@ -5786,8 +5807,11 @@
       <c r="D182" s="47" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="183" spans="1:4">
+      <c r="F182" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183">
         <f>A182+1</f>
         <v>182</v>
@@ -5802,8 +5826,11 @@
       <c r="D183" s="47" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="184" spans="1:4">
+      <c r="F183" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
       <c r="A184">
         <f>A183+1</f>
         <v>183</v>
@@ -5817,8 +5844,11 @@
       <c r="D184" s="47" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="185" spans="1:4">
+      <c r="F184" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
       <c r="A185">
         <f>A184+1</f>
         <v>184</v>
@@ -5833,8 +5863,11 @@
       <c r="D185" s="47" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="186" spans="1:4">
+      <c r="F185" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
       <c r="A186">
         <f>A185+1</f>
         <v>185</v>
@@ -5849,8 +5882,11 @@
       <c r="D186" s="47" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="187" spans="1:4">
+      <c r="F186" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
       <c r="A187">
         <f>A186+1</f>
         <v>186</v>
@@ -5865,8 +5901,11 @@
       <c r="D187" s="47" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="188" spans="1:4">
+      <c r="F187" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
       <c r="A188">
         <f>A187+1</f>
         <v>187</v>
@@ -5881,8 +5920,11 @@
       <c r="D188" s="47" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="189" spans="1:4">
+      <c r="F188" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
       <c r="A189">
         <f>A188+1</f>
         <v>188</v>
@@ -5897,8 +5939,11 @@
       <c r="D189" s="47" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="190" spans="1:4">
+      <c r="F189" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
       <c r="A190">
         <f>A189+1</f>
         <v>189</v>
@@ -5913,8 +5958,11 @@
       <c r="D190" s="47" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="191" spans="1:4">
+      <c r="F190" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191">
         <f>A190+1</f>
         <v>190</v>
@@ -5929,8 +5977,11 @@
       <c r="D191" s="47" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="192" spans="1:4">
+      <c r="F191" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
       <c r="A192">
         <f>A191+1</f>
         <v>191</v>
@@ -5945,8 +5996,11 @@
       <c r="D192" s="47" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="193" spans="1:4">
+      <c r="F192" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193">
         <f>A192+1</f>
         <v>192</v>
@@ -5960,8 +6014,11 @@
       <c r="D193" s="47" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="F193" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194">
         <f>A193+1</f>
         <v>193</v>
@@ -5976,8 +6033,11 @@
       <c r="D194" s="47" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="195" spans="1:4">
+      <c r="F194" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195">
         <f>A194+1</f>
         <v>194</v>
@@ -5992,8 +6052,11 @@
       <c r="D195" s="47" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="196" spans="1:4">
+      <c r="F195" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196">
         <f>A195+1</f>
         <v>195</v>
@@ -6008,8 +6071,11 @@
       <c r="D196" s="47" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="197" spans="1:4">
+      <c r="F196" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
       <c r="A197">
         <f>A196+1</f>
         <v>196</v>
@@ -6024,8 +6090,11 @@
       <c r="D197" s="47" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="198" spans="1:4">
+      <c r="F197" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198">
         <f>A197+1</f>
         <v>197</v>
@@ -6040,8 +6109,11 @@
       <c r="D198" s="47" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="199" spans="1:4">
+      <c r="F198" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199">
         <f>A198+1</f>
         <v>198</v>
@@ -6056,8 +6128,11 @@
       <c r="D199" s="47" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="200" spans="1:4">
+      <c r="F199" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
       <c r="A200">
         <f>A199+1</f>
         <v>199</v>
@@ -6072,8 +6147,11 @@
       <c r="D200" s="47" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="201" spans="1:4">
+      <c r="F200" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
       <c r="A201">
         <f>A200+1</f>
         <v>200</v>
@@ -6087,6 +6165,9 @@
       </c>
       <c r="D201" s="47" t="s">
         <v>296</v>
+      </c>
+      <c r="F201" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6094,7 +6175,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1591713358" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1600628105" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6103,16 +6184,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1591713358" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1591713358" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1591713358" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1591713358" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1600628105" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1600628105" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1600628105" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1600628105" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1591713358" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1600628105" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -6134,7 +6215,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1591713358" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1600628105" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6143,16 +6224,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1591713358" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1591713358" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1591713358" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1591713358" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1600628105" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1600628105" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1600628105" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1600628105" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1591713358" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1600628105" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -6174,7 +6255,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1591713358" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1600628105" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6183,16 +6264,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1591713358" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1591713358" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1591713358" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1591713358" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1600628105" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1600628105" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1600628105" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1600628105" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1591713358" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1600628105" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>